<commit_message>
Cambios en la plantilla de tiempo y limpieza del código
</commit_message>
<xml_diff>
--- a/public/plantillas/tiempos.xlsx
+++ b/public/plantillas/tiempos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eval-us-app\public\plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garconde\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659DF722-B6A4-4A03-9DA9-E7C0EFE895EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD77081-1288-413F-B2EE-AFD3C801FBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B701D779-1980-41D1-A69A-46442355D745}"/>
   </bookViews>
@@ -561,7 +561,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEBF7A00-7A7B-4E77-B892-4E0E23116618}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -592,13 +594,13 @@
     </row>
     <row r="3" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
       </c>
       <c r="C3" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -609,7 +611,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -620,29 +622,29 @@
         <v>7</v>
       </c>
       <c r="C5" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>